<commit_message>
after integratio in Rotal with Shalom. add vent process before start calib process- 16062016.
</commit_message>
<xml_diff>
--- a/base_config.xlsx
+++ b/base_config.xlsx
@@ -647,7 +647,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +731,7 @@
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5">
         <v>25.6</v>
@@ -748,22 +748,20 @@
         <v>0.34</v>
       </c>
       <c r="H8" s="5">
-        <v>25.6</v>
+        <v>28</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G9" s="4">
         <v>0.7</v>
       </c>
-      <c r="H9" s="5">
-        <v>25.6</v>
-      </c>
+      <c r="H9" s="5"/>
       <c r="J9" s="12" t="s">
         <v>6</v>
       </c>
@@ -792,7 +790,7 @@
         <v>10</v>
       </c>
       <c r="K11" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>